<commit_message>
adding file with embryo+endosperm weights determined from my species
</commit_message>
<xml_diff>
--- a/data/embryo_endosperm_weights.xlsx
+++ b/data/embryo_endosperm_weights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>GRSP</t>
   </si>
@@ -42,6 +42,18 @@
   </si>
   <si>
     <t>BOLE</t>
+  </si>
+  <si>
+    <t>BAER</t>
+  </si>
+  <si>
+    <t>PEPU</t>
+  </si>
+  <si>
+    <t>GRBU</t>
+  </si>
+  <si>
+    <t>species</t>
   </si>
 </sst>
 </file>
@@ -359,65 +371,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B18" sqref="B18:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>13.012</v>
+        <v>23.463999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>13.939</v>
+        <v>24.664999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>7.7640000000000002</v>
+        <v>2.004</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>8.5879999999999992</v>
+        <v>2.1859999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>14.329000000000001</v>
+        <v>0.82699999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>14.455</v>
+        <v>0.65700000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -425,42 +443,109 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.82699999999999996</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>2.004</v>
+        <v>26.265000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>2.1859999999999999</v>
+        <v>28.085999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>0.65700000000000003</v>
+        <v>25.745000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>0.57499999999999996</v>
+        <v>13.012</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>13.939</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>7.7640000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>8.5879999999999992</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>14.329000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>14.455</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>2.028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>2.3820000000000001</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B20">
+    <sortCondition ref="A2:A20"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>